<commit_message>
update models & documentation
</commit_message>
<xml_diff>
--- a/WP1/T1-1/geobasisdaten_filtered.xlsx
+++ b/WP1/T1-1/geobasisdaten_filtered.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hessoit-my.sharepoint.com/personal/maxime_collombi_hes-so_ch/Documents/Bureau/FGDM4GS/WP1/T1-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AD74FA93-95A4-4A67-8DC4-0621DB4DC150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB7DE1D4-A791-48E8-A2CB-8C32E7249949}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{AD74FA93-95A4-4A67-8DC4-0621DB4DC150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9883BF-8009-40E2-B8DF-F0E4665DCFD9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26625" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30135" windowHeight="20490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -390,6 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -513,13 +514,17 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau3" displayName="Tableau3" ref="A1:J31">
   <autoFilter ref="A1:J31" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="16.1;_x000a_17.1"/>
+        <filter val="72.1"/>
+        <filter val="76.1"/>
+        <filter val="86.1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="6">
       <filters>
         <filter val="xlsx"/>
@@ -770,26 +775,26 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -821,7 +826,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -850,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -879,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -908,7 +913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -937,7 +942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -966,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
@@ -995,7 +1000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1024,7 +1029,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1056,7 +1061,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1088,7 +1093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1146,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
@@ -1175,7 +1180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +1209,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
@@ -1233,7 +1238,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
@@ -1323,7 +1328,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
@@ -1410,7 +1415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>38</v>
       </c>
@@ -1439,7 +1444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1468,7 +1473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>38</v>
       </c>
@@ -1484,7 +1489,7 @@
       <c r="E24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="15" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="9" t="s">
@@ -1497,7 +1502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>38</v>
       </c>
@@ -1526,7 +1531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>38</v>
       </c>
@@ -1548,14 +1553,14 @@
       <c r="G26" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>38</v>
       </c>
@@ -1587,7 +1592,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>54</v>
       </c>
@@ -1648,7 +1653,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
@@ -1675,7 +1680,7 @@
       </c>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>58</v>
       </c>

</xml_diff>